<commit_message>
Added a new class
</commit_message>
<xml_diff>
--- a/first_basic_framework_26092015/ExcelTestData/LoginTestData.xlsx
+++ b/first_basic_framework_26092015/ExcelTestData/LoginTestData.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="login_data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -18,9 +18,35 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Test for valid username and valid password</t>
+  </si>
+  <si>
+    <t>234dotus@gmail.com</t>
+  </si>
+  <si>
+    <t>password123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Scenario Name </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="16"/>
       <color theme="1"/>
@@ -28,13 +54,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,13 +86,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -382,12 +426,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="33.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Added Excel Spreadsheet for keeping some parameters
</commit_message>
<xml_diff>
--- a/first_basic_framework_26092015/ExcelTestData/LoginTestData.xlsx
+++ b/first_basic_framework_26092015/ExcelTestData/LoginTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="12">
   <si>
     <t>Username</t>
   </si>
@@ -40,13 +40,29 @@
   </si>
   <si>
     <t xml:space="preserve">Test Scenario Name </t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Test for valid username and invalid password</t>
+  </si>
+  <si>
+    <t>Test for invalid username and valid password</t>
+  </si>
+  <si>
+    <t>haguse@gmail.com</t>
+  </si>
+  <si>
+    <t>password124</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="16"/>
       <color theme="1"/>
@@ -426,18 +442,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="33.88671875" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="33.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -464,10 +480,43 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3:B4" r:id="rId2" display="234dotus@gmail.com"/>
+    <hyperlink ref="B4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>